<commit_message>
recognizing where the diff is and canvas it
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No significant differences detected between login_home_page_20240719-123051.png and login_home_page_20240719-123231.png.</t>
+          <t>No significant differences detected between overview_home_page_20240721-155359.png and overview_home_page_20240721-155448.png.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-19 12:32:38</t>
+          <t>2024-07-21 15:55:10</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,24 +502,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0.59%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>login_home_page_20240719-123051.png</t>
+          <t>overview_home_page_20240721-155359.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>login_home_page_20240719-123231.png</t>
+          <t>overview_home_page_20240721-155448.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>No significant differences detected between login_logged_in_20240719-123056.png and login_logged_in_20240719-123236.png.</t>
+          <t>No significant differences detected between login_home_page_20240721-155402.png and login_home_page_20240721-155451.png.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-07-19 12:32:39</t>
+          <t>2024-07-21 15:55:10</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,17 +539,91 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.00%</t>
+          <t>0.60%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>login_logged_in_20240719-123056.png</t>
+          <t>login_home_page_20240721-155402.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>login_logged_in_20240719-123236.png</t>
+          <t>login_home_page_20240721-155451.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>No significant differences detected between login_logged_in_20240721-155405.png and login_logged_in_20240721-155455.png.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-07-21 15:55:10</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>1.98%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>login_logged_in_20240721-155405.png</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>login_logged_in_20240721-155455.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>No significant differences detected between overview_displayed_20240721-155418.png and overview_displayed_20240721-155507.png.</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-07-21 15:55:11</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>1.98%</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>overview_displayed_20240721-155418.png</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>overview_displayed_20240721-155507.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a JSON file to facilitate data entry.
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No significant differences detected between overview_home_page_20240721-155359.png and overview_home_page_20240721-155448.png.</t>
+          <t>No significant differences detected between overview_home_page_20240721-155448.png and overview_home_page_20240803-143929.png.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-07-21 15:55:10</t>
+          <t>2024-08-03 14:39:56</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,24 +502,24 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.59%</t>
+          <t>2.22%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>overview_home_page_20240721-155359.png</t>
+          <t>overview_home_page_20240721-155448.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>overview_home_page_20240721-155448.png</t>
+          <t>overview_home_page_20240803-143929.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>No significant differences detected between login_home_page_20240721-155402.png and login_home_page_20240721-155451.png.</t>
+          <t>No significant differences detected between login_home_page_20240721-155451.png and login_home_page_20240803-143934.png.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -529,7 +529,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-07-21 15:55:10</t>
+          <t>2024-08-03 14:39:56</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,91 +539,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.60%</t>
+          <t>2.22%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>login_home_page_20240721-155402.png</t>
+          <t>login_home_page_20240721-155451.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>login_home_page_20240721-155451.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>No significant differences detected between login_logged_in_20240721-155405.png and login_logged_in_20240721-155455.png.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2024-07-21 15:55:10</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Master</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1.98%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>login_logged_in_20240721-155405.png</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>login_logged_in_20240721-155455.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>No significant differences detected between overview_displayed_20240721-155418.png and overview_displayed_20240721-155507.png.</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Success</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2024-07-21 15:55:11</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Master</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1.98%</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>overview_displayed_20240721-155418.png</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>overview_displayed_20240721-155507.png</t>
+          <t>login_home_page_20240803-143934.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Custom data and default data added
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -482,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No significant differences detected between overview_home_page_20240721-155448.png and overview_home_page_20240803-143929.png.</t>
+          <t>No significant differences detected between test_user_registration_start.png_20240805-214011.png and test_user_registration_start.png_20240805-215315.png.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-08-03 14:39:56</t>
+          <t>2024-08-05 21:53:33</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,34 +502,34 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2.22%</t>
+          <t>0.05%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>overview_home_page_20240721-155448.png</t>
+          <t>test_user_registration_start.png_20240805-214011.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>overview_home_page_20240803-143929.png</t>
+          <t>test_user_registration_start.png_20240805-215315.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>No significant differences detected between login_home_page_20240721-155451.png and login_home_page_20240803-143934.png.</t>
+          <t>Differences detected in register: test_user_registration_end.png_20240805-214026.png vs test_user_registration_end.png_20240805-215331.png</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>Failure</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-08-03 14:39:56</t>
+          <t>2024-08-05 21:53:34</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,17 +539,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2.22%</t>
+          <t>52.99%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>login_home_page_20240721-155451.png</t>
+          <t>test_user_registration_end.png_20240805-214026.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>login_home_page_20240803-143934.png</t>
+          <t>test_user_registration_end.png_20240805-215331.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added a ui form to enter data for cutomized one
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No significant differences detected between test_user_registration_start.png_20240805-214011.png and test_user_registration_start.png_20240805-215315.png.</t>
+          <t>No significant differences detected between register_clicked_register.png_20240807-092154.png and register_clicked_register.png_20240807-095206.png.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-08-05 21:53:33</t>
+          <t>2024-08-07 09:52:25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,34 +502,34 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.05%</t>
+          <t>1.97%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>test_user_registration_start.png_20240805-214011.png</t>
+          <t>register_clicked_register.png_20240807-092154.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>test_user_registration_start.png_20240805-215315.png</t>
+          <t>register_clicked_register.png_20240807-095206.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Differences detected in register: test_user_registration_end.png_20240805-214026.png vs test_user_registration_end.png_20240805-215331.png</t>
+          <t>No significant differences detected between register_filled_form.png_20240807-092157.png and register_filled_form.png_20240807-095209.png.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Failure</t>
+          <t>Success</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-08-05 21:53:34</t>
+          <t>2024-08-07 09:52:25</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,17 +539,54 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>52.99%</t>
+          <t>0.33%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>test_user_registration_end.png_20240805-214026.png</t>
+          <t>register_filled_form.png_20240807-092157.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>test_user_registration_end.png_20240805-215331.png</t>
+          <t>register_filled_form.png_20240807-095209.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>No significant differences detected between register_submitted.png_20240807-092211.png and register_submitted.png_20240807-095222.png.</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Success</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-08-07 09:52:25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0.09%</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>register_submitted.png_20240807-092211.png</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>register_submitted.png_20240807-095222.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ui to enter  custom data
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -482,17 +482,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>No significant differences detected between register_clicked_register.png_20240807-092154.png and register_clicked_register.png_20240807-095206.png.</t>
+          <t>Differences detected in register: register_clicked_register.png_20240807-234144.png vs register_clicked_register.png_20240808-020447.png</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>Failure</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-08-07 09:52:25</t>
+          <t>2024-08-08 02:05:09</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,34 +502,34 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1.97%</t>
+          <t>23.21%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>register_clicked_register.png_20240807-092154.png</t>
+          <t>register_clicked_register.png_20240807-234144.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>register_clicked_register.png_20240807-095206.png</t>
+          <t>register_clicked_register.png_20240808-020447.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>No significant differences detected between register_filled_form.png_20240807-092157.png and register_filled_form.png_20240807-095209.png.</t>
+          <t>Differences detected in register: register_filled_form.png_20240807-234147.png vs register_filled_form.png_20240808-020451.png</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>Failure</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-08-07 09:52:25</t>
+          <t>2024-08-08 02:05:09</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,34 +539,34 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.33%</t>
+          <t>11.59%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>register_filled_form.png_20240807-092157.png</t>
+          <t>register_filled_form.png_20240807-234147.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>register_filled_form.png_20240807-095209.png</t>
+          <t>register_filled_form.png_20240808-020451.png</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>No significant differences detected between register_submitted.png_20240807-092211.png and register_submitted.png_20240807-095222.png.</t>
+          <t>Differences detected in register: register_submitted.png_20240807-234200.png vs register_submitted.png_20240808-020506.png</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Success</t>
+          <t>Failure</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2024-08-07 09:52:25</t>
+          <t>2024-08-08 02:05:09</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -576,17 +576,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.09%</t>
+          <t>57.25%</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>register_submitted.png_20240807-092211.png</t>
+          <t>register_submitted.png_20240807-234200.png</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>register_submitted.png_20240807-095222.png</t>
+          <t>register_submitted.png_20240808-020506.png</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
steps to enter custom data
</commit_message>
<xml_diff>
--- a/test_report.xlsx
+++ b/test_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,17 +482,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Differences detected in register: register_clicked_register.png_20240807-234144.png vs register_clicked_register.png_20240808-020447.png</t>
+          <t>No significant differences detected between login_home_page_20240808-092825.png and login_home_page_20240808-093030.png.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Failure</t>
+          <t>Success</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2024-08-08 02:05:09</t>
+          <t>2024-08-08 09:30:48</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -502,34 +502,34 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>23.21%</t>
+          <t>0.64%</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>register_clicked_register.png_20240807-234144.png</t>
+          <t>login_home_page_20240808-092825.png</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>register_clicked_register.png_20240808-020447.png</t>
+          <t>login_home_page_20240808-093030.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Differences detected in register: register_filled_form.png_20240807-234147.png vs register_filled_form.png_20240808-020451.png</t>
+          <t>No significant differences detected between login_error_timeout_20240808-092842.png and login_error_timeout_20240808-093045.png.</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Failure</t>
+          <t>Success</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2024-08-08 02:05:09</t>
+          <t>2024-08-08 09:30:48</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -539,54 +539,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>11.59%</t>
+          <t>1.97%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>register_filled_form.png_20240807-234147.png</t>
+          <t>login_error_timeout_20240808-092842.png</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>register_filled_form.png_20240808-020451.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Differences detected in register: register_submitted.png_20240807-234200.png vs register_submitted.png_20240808-020506.png</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Failure</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2024-08-08 02:05:09</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Master</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>57.25%</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>register_submitted.png_20240807-234200.png</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>register_submitted.png_20240808-020506.png</t>
+          <t>login_error_timeout_20240808-093045.png</t>
         </is>
       </c>
     </row>

</xml_diff>